<commit_message>
Refactor date handling and improve Excel export formatting in timesheet comparison
</commit_message>
<xml_diff>
--- a/sap.xlsx
+++ b/sap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/satyamvats/Documents/ioco/poc/timesheet-comparator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208AA06E-83F8-F341-8C20-134870BC9F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697B813D-C60F-8C48-8B5B-BDDBBDACBA59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32000" yWindow="780" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -143,21 +143,12 @@
     <t>3142477</t>
   </si>
   <si>
-    <t>Prateek Dhawan</t>
-  </si>
-  <si>
     <t>3143927</t>
   </si>
   <si>
-    <t>Vijay Thapak</t>
-  </si>
-  <si>
     <t>3144292</t>
   </si>
   <si>
-    <t>Rishi Tiwari</t>
-  </si>
-  <si>
     <t>akash.barman@nagarro.com</t>
   </si>
   <si>
@@ -165,6 +156,15 @@
   </si>
   <si>
     <t>akash.malhotra@nagarro.com</t>
+  </si>
+  <si>
+    <t>Adresh Varsney</t>
+  </si>
+  <si>
+    <t>Akash Malhotra</t>
+  </si>
+  <si>
+    <t>Akash Barman</t>
   </si>
 </sst>
 </file>
@@ -254,13 +254,13 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -602,7 +602,7 @@
   <dimension ref="A1:AC24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -615,10 +615,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
@@ -661,10 +661,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="8"/>
+      <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -683,10 +683,10 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="9"/>
     </row>
     <row r="13" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -732,86 +732,86 @@
       <c r="A19" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="8" t="s">
         <v>24</v>
       </c>
       <c r="E19" s="1"/>
-      <c r="F19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="N19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="P19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="S19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="T19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="U19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="V19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="W19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="X19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="Z19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="AB19" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC19" s="7" t="s">
+      <c r="F19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="R19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="S19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="T19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="U19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="V19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="W19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="X19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB19" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC19" s="8" t="s">
         <v>25</v>
       </c>
     </row>
@@ -819,13 +819,13 @@
       <c r="A20" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="8" t="s">
         <v>12</v>
       </c>
       <c r="E20" s="1"/>
@@ -992,20 +992,20 @@
       </c>
     </row>
     <row r="22" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
+      <c r="A22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>37</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="6">
@@ -1073,20 +1073,20 @@
       <c r="AC22" s="5"/>
     </row>
     <row r="23" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
+      <c r="A23" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>38</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -1154,20 +1154,20 @@
       </c>
     </row>
     <row r="24" spans="1:29" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="8" t="s">
         <v>32</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>39</v>
+        <v>41</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>36</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="6">
@@ -1240,6 +1240,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="F19:AC19"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="A22:A24"/>
     <mergeCell ref="B22:B24"/>
@@ -1247,7 +1248,6 @@
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="B19:D19"/>
-    <mergeCell ref="F19:AC19"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="E23" r:id="rId1" xr:uid="{B9C9D01C-2582-BD40-9AF0-C08C63E9D55F}"/>

</xml_diff>